<commit_message>
vendor archive time selected column hide and dialog check import ui and api implement
</commit_message>
<xml_diff>
--- a/new-invoice-frontend/main/src/assets/files/importcostcode.xlsx
+++ b/new-invoice-frontend/main/src/assets/files/importcostcode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\rovuk-invoice\new-invoice-frontend\main\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>cost_code</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>test for bulk import api</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
   <si>
     <t>test cost code</t>
@@ -554,7 +551,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,13 +576,11 @@
       <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -596,9 +591,7 @@
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
-        <v>10</v>
-      </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>

</xml_diff>